<commit_message>
Add parachute servo interface Update weight info and simulation file
</commit_message>
<xml_diff>
--- a/hw/Data/Mechanical_Info.xlsx
+++ b/hw/Data/Mechanical_Info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Component</t>
   </si>
@@ -57,14 +57,28 @@
   </si>
   <si>
     <t>800 mAh LiPo</t>
+  </si>
+  <si>
+    <t>Thruster Mass</t>
+  </si>
+  <si>
+    <t>Printed Thruster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,6 +135,21 @@
     <tableColumn id="2" name="Unit Mass (g)"/>
     <tableColumn id="4" name="Mass (g)">
       <calculatedColumnFormula>Table1[Unit Mass (g)]*Table1[Qty]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A16:D22" totalsRowShown="0">
+  <autoFilter ref="A16:D22"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Component"/>
+    <tableColumn id="3" name="Qty"/>
+    <tableColumn id="2" name="Unit Mass (g)"/>
+    <tableColumn id="4" name="Mass (g)">
+      <calculatedColumnFormula>Table13[Unit Mass (g)]*Table13[Qty]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -389,16 +419,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,10 +543,85 @@
         <v>178.8</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>26.5</v>
+      </c>
+      <c r="D18">
+        <f>Table13[Unit Mass (g)]*Table13[Qty]</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <f>Table13[Unit Mass (g)]*Table13[Qty]</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>71</v>
+      </c>
+      <c r="D20">
+        <f>Table13[[#This Row],[Qty]]*Table13[[#This Row],[Unit Mass (g)]]</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <f>SUM(Table13[Mass (g)])</f>
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>